<commit_message>
EPBDS-6933 VarArg does not work properly.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/binding/VarArgsMethodBindingTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/binding/VarArgsMethodBindingTest.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\binding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>return anyTrue(true, false);</t>
   </si>
@@ -70,12 +75,31 @@
   <si>
     <t>Method boolean test2Arguments()</t>
   </si>
+  <si>
+    <t>Method int test4Arguments()</t>
+  </si>
+  <si>
+    <t>Method int test4(Object[] args)</t>
+  </si>
+  <si>
+    <t>return args.length;</t>
+  </si>
+  <si>
+    <t>return test4((Integer) 5, "abc", (Integer) 10, (Integer) 12, (Double) 14);</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,24 +161,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -201,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +266,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +318,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -442,118 +511,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="7" max="7" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="47" style="4" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="44.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="1" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="72.75" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-7380 Bug in varargs functionality
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/binding/VarArgsMethodBindingTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/binding/VarArgsMethodBindingTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>return anyTrue(true, false);</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>Method int test5(int a, String b, DoubleValue[] c)</t>
+  </si>
+  <si>
+    <t>test case 6</t>
+  </si>
+  <si>
+    <t>Method int test6(int a, String b, Double[] c)</t>
+  </si>
+  <si>
+    <t>Method int test6Arguments()</t>
+  </si>
+  <si>
+    <t>return test6(5, "abc", 10, (long) 12, (double) 14);</t>
   </si>
 </sst>
 </file>
@@ -183,11 +195,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -528,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +557,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1"/>
@@ -554,18 +566,18 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
@@ -580,7 +592,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1"/>
       <c r="C7" s="5" t="s">
         <v>1</v>
@@ -593,7 +605,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
@@ -608,7 +620,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="6" t="s">
         <v>8</v>
@@ -621,7 +633,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1"/>
@@ -630,14 +642,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="1"/>
@@ -652,7 +664,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
         <v>19</v>
@@ -665,24 +677,24 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1"/>
@@ -692,8 +704,37 @@
         <v>6</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A6:A7"/>

</xml_diff>